<commit_message>
Updating the Readme file
</commit_message>
<xml_diff>
--- a/ETL Mapping document.xlsx
+++ b/ETL Mapping document.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\DataClass\Pokemon_friends\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ff7e871eabf9cc2/Desktop/dataclass/UCI-VIRT-DATA-PT-11-2021-U-C/Projects/Project ^N2/Pokemon_friends/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02526D43-557F-4D0F-B60E-D14C7B0AFF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33915" yWindow="675" windowWidth="25215" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -323,18 +323,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,22 +555,22 @@
   </sheetPr>
   <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N56" sqref="N56"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="18.54296875" customWidth="1"/>
-    <col min="3" max="3" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="9" max="9" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.54296875" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -598,7 +598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -616,12 +616,12 @@
       <c r="H4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="18" t="s">
         <v>23</v>
       </c>
       <c r="J4" s="14"/>
     </row>
-    <row r="5" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -630,7 +630,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="9" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -643,7 +643,7 @@
       <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="15"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="3" t="s">
@@ -663,12 +663,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
     </row>
-    <row r="11" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -700,7 +700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>1</v>
       </c>
@@ -732,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>1</v>
       </c>
@@ -764,7 +764,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -796,7 +796,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <v>1</v>
       </c>
@@ -828,7 +828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -860,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>1</v>
       </c>
@@ -892,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>1</v>
       </c>
@@ -924,7 +924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <v>1</v>
       </c>
@@ -956,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
         <v>1</v>
       </c>
@@ -988,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
@@ -1009,7 +1009,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -1030,17 +1030,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
     </row>
-    <row r="24" spans="1:14" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
     </row>
-    <row r="25" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
@@ -1051,13 +1051,13 @@
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
     </row>
-    <row r="26" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
       <c r="E26" s="6" t="s">
         <v>28</v>
       </c>
@@ -1065,13 +1065,13 @@
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
     </row>
-    <row r="27" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+    <row r="27" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
       <c r="E27" s="6" t="s">
         <v>28</v>
       </c>
@@ -1079,13 +1079,13 @@
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
     </row>
-    <row r="28" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
+    <row r="28" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
       <c r="E28" s="6" t="s">
         <v>28</v>
       </c>
@@ -1093,12 +1093,12 @@
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
     </row>
-    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
     </row>
-    <row r="30" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>20</v>
       </c>
@@ -1106,7 +1106,7 @@
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="31" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>1</v>
       </c>
@@ -1118,7 +1118,7 @@
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
     </row>
-    <row r="32" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>2</v>
       </c>
@@ -1130,12 +1130,12 @@
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
     </row>
-    <row r="33" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>3</v>
       </c>
       <c r="B33" s="5"/>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="17" t="s">
         <v>41</v>
       </c>
       <c r="D33" s="14"/>
@@ -1144,7 +1144,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
     </row>
-    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10">
         <v>4</v>
       </c>
@@ -1155,98 +1155,98 @@
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
     </row>
-    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
     </row>
-    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
     </row>
-    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
       <c r="H37" s="14"/>
     </row>
-    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
       <c r="H38" s="14"/>
     </row>
-    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F39" s="14"/>
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
     </row>
-    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
       <c r="H40" s="14"/>
     </row>
-    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F41" s="14"/>
       <c r="G41" s="14"/>
       <c r="H41" s="14"/>
     </row>
-    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F42" s="14"/>
       <c r="G42" s="14"/>
       <c r="H42" s="14"/>
     </row>
-    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
       <c r="H43" s="14"/>
     </row>
-    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
       <c r="H44" s="14"/>
     </row>
-    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
       <c r="H45" s="14"/>
     </row>
-    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F46" s="14"/>
       <c r="G46" s="14"/>
       <c r="H46" s="14"/>
     </row>
-    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F47" s="14"/>
       <c r="G47" s="14"/>
       <c r="H47" s="14"/>
     </row>
-    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F48" s="14"/>
       <c r="G48" s="14"/>
       <c r="H48" s="14"/>
     </row>
-    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F49" s="14"/>
       <c r="G49" s="14"/>
       <c r="H49" s="14"/>
     </row>
-    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F50" s="14"/>
       <c r="G50" s="14"/>
       <c r="H50" s="14"/>
     </row>
-    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F51" s="14"/>
       <c r="G51" s="14"/>
       <c r="H51" s="14"/>
     </row>
-    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F52" s="14"/>
       <c r="G52" s="14"/>
       <c r="H52" s="14"/>
     </row>
-    <row r="53" spans="1:14" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
         <v>9</v>
       </c>
@@ -1259,7 +1259,7 @@
       <c r="D53" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F53" s="15"/>
+      <c r="F53" s="13"/>
       <c r="G53" s="14"/>
       <c r="H53" s="14"/>
       <c r="I53" s="12" t="s">
@@ -1279,12 +1279,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F54" s="14"/>
       <c r="G54" s="14"/>
       <c r="H54" s="14"/>
     </row>
-    <row r="55" spans="1:14" s="11" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="10">
         <v>2</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:14" s="11" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="10">
         <v>2</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:14" s="11" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="10">
         <v>2</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:14" s="11" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="10">
         <v>2</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:14" s="11" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="10">
         <v>2</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:14" s="11" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="10">
         <v>2</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="10">
         <v>2</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="10">
         <v>2</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="10">
         <v>2</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="10">
         <v>2</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="10">
         <v>2</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="10">
         <v>2</v>
       </c>
@@ -1668,17 +1668,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F67" s="14"/>
       <c r="G67" s="14"/>
       <c r="H67" s="14"/>
     </row>
-    <row r="68" spans="1:14" s="11" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" s="11" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F68" s="14"/>
       <c r="G68" s="14"/>
       <c r="H68" s="14"/>
     </row>
-    <row r="69" spans="1:14" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>19</v>
       </c>
@@ -1689,13 +1689,13 @@
       <c r="G69" s="14"/>
       <c r="H69" s="14"/>
     </row>
-    <row r="70" spans="1:14" s="11" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="17" t="s">
+    <row r="70" spans="1:14" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
-      <c r="D70" s="17"/>
+      <c r="B70" s="15"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
       <c r="E70" s="11" t="s">
         <v>44</v>
       </c>
@@ -1703,11 +1703,11 @@
       <c r="G70" s="14"/>
       <c r="H70" s="14"/>
     </row>
-    <row r="71" spans="1:14" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="18"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
+    <row r="71" spans="1:14" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="16"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
       <c r="E71" s="11" t="s">
         <v>44</v>
       </c>
@@ -1715,11 +1715,11 @@
       <c r="G71" s="14"/>
       <c r="H71" s="14"/>
     </row>
-    <row r="72" spans="1:14" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="18"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
+    <row r="72" spans="1:14" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="16"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
       <c r="E72" s="11" t="s">
         <v>44</v>
       </c>
@@ -1727,12 +1727,12 @@
       <c r="G72" s="14"/>
       <c r="H72" s="14"/>
     </row>
-    <row r="73" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F73" s="14"/>
       <c r="G73" s="14"/>
       <c r="H73" s="14"/>
     </row>
-    <row r="74" spans="1:14" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>20</v>
       </c>
@@ -1740,7 +1740,7 @@
       <c r="G74" s="14"/>
       <c r="H74" s="14"/>
     </row>
-    <row r="75" spans="1:14" s="11" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="10">
         <v>1</v>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="G75" s="14"/>
       <c r="H75" s="14"/>
     </row>
-    <row r="76" spans="1:14" s="11" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="10">
         <v>2</v>
       </c>
@@ -1764,12 +1764,12 @@
       <c r="G76" s="14"/>
       <c r="H76" s="14"/>
     </row>
-    <row r="77" spans="1:14" s="11" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="10">
         <v>3</v>
       </c>
       <c r="B77" s="5"/>
-      <c r="C77" s="16" t="s">
+      <c r="C77" s="17" t="s">
         <v>69</v>
       </c>
       <c r="D77" s="14"/>
@@ -1778,7 +1778,7 @@
       <c r="G77" s="14"/>
       <c r="H77" s="14"/>
     </row>
-    <row r="78" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="10">
         <v>4</v>
       </c>
@@ -1789,109 +1789,109 @@
       <c r="G78" s="14"/>
       <c r="H78" s="14"/>
     </row>
-    <row r="79" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F79" s="14"/>
       <c r="G79" s="14"/>
       <c r="H79" s="14"/>
     </row>
-    <row r="80" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F80" s="14"/>
       <c r="G80" s="14"/>
       <c r="H80" s="14"/>
     </row>
-    <row r="81" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F81" s="14"/>
       <c r="G81" s="14"/>
       <c r="H81" s="14"/>
     </row>
-    <row r="82" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F82" s="14"/>
       <c r="G82" s="14"/>
       <c r="H82" s="14"/>
     </row>
-    <row r="83" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F83" s="14"/>
       <c r="G83" s="14"/>
       <c r="H83" s="14"/>
     </row>
-    <row r="84" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F84" s="14"/>
       <c r="G84" s="14"/>
       <c r="H84" s="14"/>
     </row>
-    <row r="85" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F85" s="14"/>
       <c r="G85" s="14"/>
       <c r="H85" s="14"/>
     </row>
-    <row r="86" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F86" s="14"/>
       <c r="G86" s="14"/>
       <c r="H86" s="14"/>
     </row>
-    <row r="87" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F87" s="14"/>
       <c r="G87" s="14"/>
       <c r="H87" s="14"/>
     </row>
-    <row r="88" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F88" s="14"/>
       <c r="G88" s="14"/>
       <c r="H88" s="14"/>
     </row>
-    <row r="89" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F89" s="14"/>
       <c r="G89" s="14"/>
       <c r="H89" s="14"/>
     </row>
-    <row r="90" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F90" s="14"/>
       <c r="G90" s="14"/>
       <c r="H90" s="14"/>
     </row>
-    <row r="91" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F91" s="14"/>
       <c r="G91" s="14"/>
       <c r="H91" s="14"/>
     </row>
-    <row r="92" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F92" s="14"/>
       <c r="G92" s="14"/>
       <c r="H92" s="14"/>
     </row>
-    <row r="93" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F93" s="14"/>
       <c r="G93" s="14"/>
       <c r="H93" s="14"/>
     </row>
-    <row r="94" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F94" s="14"/>
       <c r="G94" s="14"/>
       <c r="H94" s="14"/>
     </row>
-    <row r="95" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F95" s="14"/>
       <c r="G95" s="14"/>
       <c r="H95" s="14"/>
     </row>
-    <row r="96" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="6:8" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F96" s="14"/>
       <c r="G96" s="14"/>
       <c r="H96" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="F53:H96"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A72:D72"/>
-    <mergeCell ref="C77:E77"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="F9:H52"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A28:D28"/>
+    <mergeCell ref="F53:H96"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="C77:E77"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>